<commit_message>
MAJ de verif.py pour Valentin
</commit_message>
<xml_diff>
--- a/projet_ST7/phase_1/InstancesV1/InstancePolandV1.xlsx
+++ b/projet_ST7/phase_1/InstancesV1/InstancePolandV1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anne-laurencethoux/Documents/Thèse/ST_CtlSup/InstancesV1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexisrichard/Desktop/CentraleSupélec/2A/7 - ST/ST7 optimisation de transport passagers/projet DecisionBrain/projet_ST7/projet_ST7/phase_1/InstancesV1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD4D379-8C54-8741-929B-FC5BAB79C4D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C199C0F-7FF5-884A-9296-5E789A86E5B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53620" yWindow="4240" windowWidth="29260" windowHeight="15820" xr2:uid="{745759C5-7123-8144-B92E-2C75C62BB0A9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{745759C5-7123-8144-B92E-2C75C62BB0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitde</t>
   </si>
   <si>
     <t>Longitude</t>
@@ -644,78 +638,78 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -745,19 +739,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -784,522 +778,522 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1">
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
         <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1">
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1">
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1">
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1">
         <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1">
         <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1">
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1">
         <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1">
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1">
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1">
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1">
         <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1">
         <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1">
         <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1">
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1">
         <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1626,13 +1620,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>